<commit_message>
Created Slides for Questions 2-4.
</commit_message>
<xml_diff>
--- a/Data/Question3.xlsx
+++ b/Data/Question3.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Udacity\UdacityProjects\DVD_Rental_Database\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{15BF8B80-8736-4905-9BD4-F9D433CBA6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334E2B50-D2F7-4305-AD58-FE9C236E7FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="24" r:id="rId3"/>
+    <pivotCache cacheId="7" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -622,11 +622,11 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -678,11 +678,451 @@
       <c:pivotFmt>
         <c:idx val="1"/>
         <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -734,8 +1174,9 @@
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -752,17 +1193,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
               <c:f>Sheet1!$A$5:$A$11</c:f>
@@ -814,7 +1253,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0813-4AF9-844C-8CAFD53549C2}"/>
@@ -836,17 +1274,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
               <c:f>Sheet1!$A$5:$A$11</c:f>
@@ -898,7 +1334,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0813-4AF9-844C-8CAFD53549C2}"/>
@@ -913,10 +1348,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
+        <c:gapWidth val="150"/>
         <c:axId val="1795293712"/>
         <c:axId val="1795295792"/>
-      </c:lineChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="1795293712"/>
         <c:scaling>
@@ -1721,7 +2156,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="harvey" refreshedDate="44435.977768634257" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="8">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="harvey" refreshedDate="44435.977768634257" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="8" xr:uid="{00000000-000A-0000-FFFF-FFFF18000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:D9" sheet="Question3"/>
   </cacheSource>
@@ -1812,7 +2247,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable12" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable12" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:D11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -2218,11 +2653,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2231,9 +2666,13 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2363,7 +2802,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>